<commit_message>
final analysis clean up
</commit_message>
<xml_diff>
--- a/currencies_analysis/EURUSD=X_predicted_results.xlsx
+++ b/currencies_analysis/EURUSD=X_predicted_results.xlsx
@@ -5,17 +5,30 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jyin1\OneDrive\uni-hers\Projects and Competitions\Citi 24\Citi-Comp-24\currencies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jyin1\OneDrive\uni-hers\Projects and Competitions\Citi 24\Citi-Comp-24\currencies_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD67D6A-BA80-4D52-A737-1B3B41795AD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D640A81F-E876-46F0-B18E-0D2C30556ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13800" yWindow="-15870" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -45,7 +58,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="[$-C09]dd\-mmm\-yy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-C09]dd\-mmm\-yy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -101,10 +114,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,13 +422,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E539"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A514" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B268" sqref="B268:B523"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -4962,7 +4977,7 @@
         <v>43602</v>
       </c>
       <c r="B268">
-        <v>1.117355942726135</v>
+        <v>1.1173559427261399</v>
       </c>
       <c r="C268">
         <v>1.1193743332828889</v>
@@ -9263,7 +9278,7 @@
         <v>45373</v>
       </c>
       <c r="B521">
-        <v>1.086236238479614</v>
+        <v>1.08623623847961</v>
       </c>
       <c r="C521">
         <v>1.088864152982757</v>

</xml_diff>